<commit_message>
Added json config file and some more excel examples.
</commit_message>
<xml_diff>
--- a/templates/excel_template.xlsx
+++ b/templates/excel_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tr####" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -94,11 +94,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,16 +138,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,11 +166,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -224,10 +215,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -260,14 +251,14 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">

</xml_diff>